<commit_message>
Included PCE results in the log outputs and details on dataset size
</commit_message>
<xml_diff>
--- a/feature_importance_PBE_eth.xlsx
+++ b/feature_importance_PBE_eth.xlsx
@@ -448,31 +448,31 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>electronegativity</t>
+          <t>deltaE_RedOxH</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.09101712819681956</v>
+        <v>0.0852532962900039</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>HBondAcceptors</t>
+          <t>IP</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.07734396885002499</v>
+        <v>0.06734353704942037</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>deltaE_RedOxH</t>
+          <t>HOMO</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.06380083974345843</v>
+        <v>0.05530325205805955</v>
       </c>
     </row>
     <row r="5">
@@ -482,257 +482,257 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.05709373762316084</v>
+        <v>0.05459798518767987</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Max_f_osc</t>
+          <t>deltaE_LCB</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.05050618701547728</v>
+        <v>0.04825404361252158</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>LUMO</t>
+          <t>electronegativity</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.05007010553096593</v>
+        <v>0.04680774305276485</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>LHE</t>
+          <t>Max_f_osc</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.04786197888478647</v>
+        <v>0.04525695612708441</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>deltaE_LCB</t>
+          <t>electrophilicityIndex</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.04292114027776883</v>
+        <v>0.0449889657122557</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>RingCount</t>
+          <t>Surface_Area_A2</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.04145557051717391</v>
+        <v>0.04028816928167109</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>AromaticRings</t>
+          <t>Molecular_Volume_A3</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.03993979274079987</v>
+        <v>0.03867154047465479</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>IP</t>
+          <t>HBondAcceptors</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.03990060961627006</v>
+        <v>0.03714603299851457</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>electroacceptingPower</t>
+          <t>deltaE_HL</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.03709531671654899</v>
+        <v>0.03569813232664815</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Mass</t>
+          <t>LHE</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.03225239389609239</v>
+        <v>0.03287102828368097</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Max_Absorption_nm</t>
+          <t>Total_Energy_Hartree</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.02983360630176965</v>
+        <v>0.03196260193340262</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Molecular_Volume_A3</t>
+          <t>electroacceptingPower</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.02796822453169268</v>
+        <v>0.03097894467992434</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>deltaE_HL</t>
+          <t>TPSA</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.02774614733477851</v>
+        <v>0.03000586522158782</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>HOMO</t>
+          <t>chemHardness</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.02772450624476321</v>
+        <v>0.0299488781731147</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Solvation_Energy_eV</t>
+          <t>RingCount</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.0275295963926707</v>
+        <v>0.02631034166682851</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>TPSA</t>
+          <t>electrodonatingPower</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.0246741427979724</v>
+        <v>0.02476738987344099</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Total_Energy_Hartree</t>
+          <t>HBondDonors</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.02276667149408453</v>
+        <v>0.02443145326078758</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Dipole_Moment</t>
+          <t>LUMO</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.02252115700062629</v>
+        <v>0.02344892064026551</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>electrodonatingPower</t>
+          <t>Max_Absorption_nm</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.02096458338753817</v>
+        <v>0.02273387369672214</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>chemHardness</t>
+          <t>EA</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.0196090599146365</v>
+        <v>0.02182879962396833</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>LogP</t>
+          <t>AromaticRings</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.01843898906709142</v>
+        <v>0.02050164763705128</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>electrophilicityIndex</t>
+          <t>LogP</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0.01627984032914478</v>
+        <v>0.01946073814220173</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>HBondDonors</t>
+          <t>elnChemPot</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0.01496030630585054</v>
+        <v>0.01839312867180041</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>EA</t>
+          <t>Dipole_Moment</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>0.01041048539100606</v>
+        <v>0.01493344666395918</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Surface_Area_A2</t>
+          <t>Solvation_Energy_eV</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0.0102158690865171</v>
+        <v>0.01399992049796566</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>elnChemPot</t>
+          <t>Mass</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>0.007098044810510087</v>
+        <v>0.01381336716201939</v>
       </c>
     </row>
     <row r="31">

</xml_diff>